<commit_message>
Updated some minor data definitions issues
</commit_message>
<xml_diff>
--- a/dataDefinitions.xlsx
+++ b/dataDefinitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ss2302/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0A27FE-F671-5546-B729-82BA3ED1960D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484E6207-5AC9-4296-82DE-479D2F9EF244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="220" windowWidth="27780" windowHeight="18900" xr2:uid="{3F3756E1-F16D-4C67-A02C-119F78A23B8F}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3F3756E1-F16D-4C67-A02C-119F78A23B8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Imaging" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="276">
   <si>
     <t>File name</t>
   </si>
@@ -288,9 +288,6 @@
     <t>planes.delay</t>
   </si>
   <si>
-    <t>planes.zcorrStack</t>
-  </si>
-  <si>
     <t>planes.zTrace</t>
   </si>
   <si>
@@ -1006,9 +1003,6 @@
   </si>
   <si>
     <t>circles.endTime</t>
-  </si>
-  <si>
-    <t>Dimensions swapped. Should be [numROIs x numZStackPlanes]</t>
   </si>
   <si>
     <r>
@@ -1027,9 +1021,6 @@
     <t>zstack.correlation</t>
   </si>
   <si>
-    <t>This is unrelated to the imaged planes. Dimensions do not match. Rename to zstack.correlations</t>
-  </si>
-  <si>
     <t>nFrames, nROIs</t>
   </si>
   <si>
@@ -1039,27 +1030,32 @@
     <t>nROIs, nZStackPlanes</t>
   </si>
   <si>
-    <t>nZStackPlanes, nFrames</t>
-  </si>
-  <si>
-    <r>
-      <t>ID of each ROI (match IDs returned by suite2p)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>, currently saved as calcium.Ids</t>
-    </r>
+    <t>plane number</t>
+  </si>
+  <si>
+    <t>The plane in the z-stack the each plane is one for each imaging frame</t>
+  </si>
+  <si>
+    <t>luminance</t>
+  </si>
+  <si>
+    <t>ID of each ROI (match IDs returned by suite2p)</t>
+  </si>
+  <si>
+    <t>The luminance of each ROI on each slice of the z-stack</t>
+  </si>
+  <si>
+    <t>nplanes,nZStackPlanes, nFrames</t>
+  </si>
+  <si>
+    <t>The correlation of each plane with the zstack plane in each frame</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1116,8 +1112,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1139,12 +1141,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1220,11 +1216,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1631,23 +1629,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C25F9AC-6BF1-4115-A50A-42D1CDBFF915}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="157.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="20.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="157.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="8" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1661,7 +1659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1669,13 +1667,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1683,17 +1681,17 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -1707,27 +1705,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="D6" s="14" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="15" t="s">
+        <v>269</v>
+      </c>
       <c r="C7" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="D7" s="17"/>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1740,8 +1733,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1751,10 +1744,10 @@
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1765,10 +1758,10 @@
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1782,63 +1775,72 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="B13" s="17"/>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>271</v>
+      </c>
       <c r="C13" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D13" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30">
+      <c r="A15" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B15" s="17"/>
+      <c r="B15" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="C15" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D15" s="17"/>
-    </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="D16" s="14"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    </row>
+    <row r="24" spans="1:4" ht="90">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B23" r:id="rId1" xr:uid="{9251FEBC-1780-407A-BF75-F4B5997F5A88}"/>
+    <hyperlink ref="B24" r:id="rId1" xr:uid="{9251FEBC-1780-407A-BF75-F4B5997F5A88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>
@@ -1854,16 +1856,16 @@
       <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="157.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="20.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="157.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="8" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1877,65 +1879,65 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="10" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="10" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="10" customFormat="1">
       <c r="A4" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="10" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="10" customFormat="1">
       <c r="A6" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -1944,12 +1946,12 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="10" customFormat="1">
+      <c r="A7" s="1" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -1958,12 +1960,12 @@
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="10" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
@@ -1972,268 +1974,268 @@
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="10" customFormat="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="C12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="B13" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="6" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="30">
+      <c r="A14" s="6" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="6"/>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45">
+      <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30">
+      <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="D20" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30">
+      <c r="A21" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="1" t="s">
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="D23" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30">
+      <c r="A28" s="1" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="1" t="s">
+    </row>
+    <row r="30" spans="1:4" ht="30">
+      <c r="A30" s="1" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2251,16 +2253,16 @@
       <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="157.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="20.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="157.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="8" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2274,23 +2276,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -2299,44 +2301,44 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -2345,16 +2347,16 @@
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -2363,7 +2365,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2376,20 +2378,20 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="26.5" style="1" customWidth="1"/>
+    <col min="1" max="2" width="26.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="157.5" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="157.42578125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2403,495 +2405,495 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" s="7" customFormat="1"/>
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30">
+      <c r="A15" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="E15" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D17" s="11">
         <v>4</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="7" customFormat="1"/>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
     </row>
-    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="B25" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D25" s="2" t="s">
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="45">
       <c r="A32" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" s="1" t="s">
+    </row>
+    <row r="33" spans="1:5" ht="90">
+      <c r="A33" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="B33" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C33" s="13">
         <v>4</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="150">
       <c r="A37" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D41" s="1" t="s">
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="B42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="B43" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D43" s="1" t="s">
+    </row>
+    <row r="44" spans="1:5" ht="30">
+      <c r="A44" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2905,19 +2907,19 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="157.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="20.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="157.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="8" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2931,536 +2933,536 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="10" customFormat="1">
       <c r="A2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="10" customFormat="1">
+      <c r="A3" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="10" customFormat="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="10" customFormat="1">
       <c r="A5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="10" customFormat="1">
+      <c r="A6" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="10" customFormat="1">
+      <c r="A7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="10" customFormat="1">
+      <c r="A8" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="10" customFormat="1">
+      <c r="A9" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="10" customFormat="1">
+      <c r="A10" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B20" s="1" t="s">
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:4" s="7" customFormat="1"/>
+    <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D33" s="1" t="s">
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="D37" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="B38" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D37" s="1" t="s">
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="44" spans="1:4">
+      <c r="A44" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="D44" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A46" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D44" s="1" t="s">
+      <c r="B46" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:4">
+      <c r="A47" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D46" s="1" t="s">
+      <c r="B47" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:4">
+      <c r="A48" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D47" s="1" t="s">
+      <c r="B48" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>222</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data def file
</commit_message>
<xml_diff>
--- a/dataDefinitions.xlsx
+++ b/dataDefinitions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspaces\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727FAC88-D3B0-4C4C-A3F6-D452F2B73678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D954D0-241B-4FD4-956C-FBB041528CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3F3756E1-F16D-4C67-A02C-119F78A23B8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{3F3756E1-F16D-4C67-A02C-119F78A23B8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Imaging" sheetId="1" r:id="rId1"/>
@@ -213,7 +213,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="247">
   <si>
     <t>File name</t>
   </si>
@@ -500,57 +500,15 @@
     <t>Time of licks</t>
   </si>
   <si>
-    <t>grating.intervals</t>
-  </si>
-  <si>
-    <t>grating.gratingID</t>
-  </si>
-  <si>
-    <t>gratingID.direction</t>
-  </si>
-  <si>
-    <t>gratingID.spatFreq</t>
-  </si>
-  <si>
-    <t>gratingID.tempFreq</t>
-  </si>
-  <si>
-    <t>gratingID.contrast</t>
-  </si>
-  <si>
-    <t>grating.gratingExp</t>
-  </si>
-  <si>
-    <t>gratingExp.description</t>
-  </si>
-  <si>
-    <t>nTrials, 2</t>
-  </si>
-  <si>
-    <t>start and end of trial</t>
-  </si>
-  <si>
     <t xml:space="preserve">nTrials </t>
   </si>
   <si>
-    <t>ID of grating in trial</t>
-  </si>
-  <si>
     <t>nTrials</t>
   </si>
   <si>
-    <t>ID of experiment</t>
-  </si>
-  <si>
     <t>degrees</t>
   </si>
   <si>
-    <t>nGratings</t>
-  </si>
-  <si>
-    <t>direction of movement of grating; 0 -&gt; moving rightward, &gt;0 -&gt; away from zero in anti-clockwise direction</t>
-  </si>
-  <si>
     <t>cycles/degree</t>
   </si>
   <si>
@@ -563,69 +521,15 @@
     <t>temporal frequency</t>
   </si>
   <si>
-    <t>percent</t>
-  </si>
-  <si>
     <t>contrast</t>
   </si>
   <si>
-    <t>nExperiments</t>
-  </si>
-  <si>
-    <t>json; text description of experiment</t>
-  </si>
-  <si>
-    <t>sparseNoise.times</t>
-  </si>
-  <si>
-    <t>sparseNoise.map</t>
-  </si>
-  <si>
-    <t>sparseNoiseArea.edges</t>
-  </si>
-  <si>
-    <t>time of each sparse noise frame</t>
-  </si>
-  <si>
     <t>nFrames</t>
   </si>
   <si>
-    <t>nFrames, nRows, nColumns</t>
-  </si>
-  <si>
-    <t>double [-1 1]</t>
-  </si>
-  <si>
-    <t>gray value of each pixel in each stimulus frame, -1 -&gt; black, +1 -&gt; white</t>
-  </si>
-  <si>
     <t>Left, right, bottom, top edge of each stimulus frame relative to visual field. 0 -&gt; horizon/midline</t>
   </si>
   <si>
-    <t>darkScreen.intervals</t>
-  </si>
-  <si>
-    <t>nIntervals, 2</t>
-  </si>
-  <si>
-    <t>start and end of recordings during darkness</t>
-  </si>
-  <si>
-    <t>grayScreen.intervals</t>
-  </si>
-  <si>
-    <t>start and end of recordings during gray screen presentation</t>
-  </si>
-  <si>
-    <t>gratingExp.intervals</t>
-  </si>
-  <si>
-    <t>nExperiments, 2</t>
-  </si>
-  <si>
-    <t>start and end of each experiment (recording time, which can be before first and after last stimulus)</t>
-  </si>
-  <si>
     <t>sync.times</t>
   </si>
   <si>
@@ -881,18 +785,12 @@
     <t>rois.zProfiles</t>
   </si>
   <si>
-    <t>Current naming</t>
-  </si>
-  <si>
     <t>start of trial</t>
   </si>
   <si>
     <t>end of trial</t>
   </si>
   <si>
-    <t>gratings.ori</t>
-  </si>
-  <si>
     <t xml:space="preserve">direction of movement </t>
   </si>
   <si>
@@ -905,12 +803,6 @@
     <t>gratings.contrast</t>
   </si>
   <si>
-    <t>sparse.st</t>
-  </si>
-  <si>
-    <t>sparse.et</t>
-  </si>
-  <si>
     <t>sparse.map</t>
   </si>
   <si>
@@ -920,12 +812,6 @@
     <t>value for each square 0 to 1 (0 black , 1 white)</t>
   </si>
   <si>
-    <t>sparseArea.edges</t>
-  </si>
-  <si>
-    <t>retinal.stim</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -980,21 +866,12 @@
     <t>a range of stimulus sizes that elicit at least half the maximum response. Rest in nan</t>
   </si>
   <si>
-    <t>fullField</t>
-  </si>
-  <si>
     <t>gratings.startTime</t>
   </si>
   <si>
     <t>gratings.endTime</t>
   </si>
   <si>
-    <t>retinal.startTime</t>
-  </si>
-  <si>
-    <t>retinal.endTime</t>
-  </si>
-  <si>
     <t>circles.startTime</t>
   </si>
   <si>
@@ -1040,7 +917,43 @@
     <t>wheel.times</t>
   </si>
   <si>
-    <t>3D position of ROIs in imaging volume. 1st: x position (horizontal) in pixels from left of FOV. 2nd: y position (vertical) in pixels from top of FOV. 3rd: depth in microns relative to imaging volume (unrelated to brain surface).</t>
+    <t>3D position of ROIs in imaging volume. 1st: x position (vertical) in pixels from left of FOV. 2nd: y position (horizontal) in pixels from top of FOV. 3rd: depth in microns relative to imaging volume (unrelated to brain surface).</t>
+  </si>
+  <si>
+    <t>gratings.direction</t>
+  </si>
+  <si>
+    <t>sparse.startTime</t>
+  </si>
+  <si>
+    <t>sparseExp.edges</t>
+  </si>
+  <si>
+    <t>gratingsExp.intervals</t>
+  </si>
+  <si>
+    <t>nSession,2</t>
+  </si>
+  <si>
+    <t>start and end time of each session</t>
+  </si>
+  <si>
+    <t>sparseExp.intervals</t>
+  </si>
+  <si>
+    <t>fullField.startTime</t>
+  </si>
+  <si>
+    <t>fullField.endTime</t>
+  </si>
+  <si>
+    <t>fullField.stim</t>
+  </si>
+  <si>
+    <t>fullFieldExp.intervals</t>
+  </si>
+  <si>
+    <t>circlesExp.intervals</t>
   </si>
 </sst>
 </file>
@@ -1106,18 +1019,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1161,7 +1068,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1169,11 +1076,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1194,7 +1097,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1209,6 +1112,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1618,9 +1525,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C25F9AC-6BF1-4115-A50A-42D1CDBFF915}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="A30:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,54 +1539,54 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="A4" s="14"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1688,7 +1595,7 @@
       <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1696,18 +1603,18 @@
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>266</v>
+      <c r="B7" s="13" t="s">
+        <v>225</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>264</v>
+        <v>223</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>267</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1716,7 +1623,7 @@
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1730,12 +1637,12 @@
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>269</v>
+      <c r="D10" s="14" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1744,12 +1651,12 @@
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>275</v>
+      <c r="D11" s="14" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1764,37 +1671,37 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>268</v>
+        <v>227</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>270</v>
+        <v>224</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>262</v>
+        <v>221</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>271</v>
+        <v>230</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>272</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D16" s="14"/>
+      <c r="D16" s="12"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1821,7 +1728,7 @@
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1852,140 +1759,140 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1994,12 +1901,12 @@
       <c r="C11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2008,7 +1915,7 @@
       <c r="C12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2022,12 +1929,12 @@
       <c r="C13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2036,15 +1943,15 @@
       <c r="C14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
+      <c r="A15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2053,7 +1960,7 @@
       <c r="C16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2237,7 +2144,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="A1:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2249,23 +2156,23 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>273</v>
+        <v>232</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>85</v>
@@ -2279,7 +2186,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>274</v>
+        <v>233</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -2362,11 +2269,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F47D32-613F-478F-B67D-600975316B20}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2378,501 +2285,340 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>106</v>
+      <c r="D3" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>98</v>
+        <v>195</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>113</v>
+        <v>96</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>99</v>
+      <c r="A8" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>102</v>
+        <v>236</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>197</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="11">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>120</v>
+        <v>241</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>124</v>
+        <v>239</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>122</v>
+        <v>243</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="11">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>129</v>
+        <v>245</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>130</v>
+        <v>239</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>133</v>
+      <c r="C21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
+      <c r="A22" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>256</v>
+        <v>201</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>257</v>
+        <v>203</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>226</v>
+        <v>95</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>112</v>
+        <v>207</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>113</v>
+        <v>96</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C33" s="13">
-        <v>4</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>240</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -2884,9 +2630,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DAE84D7-1D35-455E-9EAE-38426D5ED717}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2898,550 +2644,550 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>174</v>
+        <v>142</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D13" s="6"/>
+        <v>128</v>
+      </c>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>178</v>
+        <v>146</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D14" s="6"/>
+        <v>124</v>
+      </c>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D15" s="6"/>
+        <v>124</v>
+      </c>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>181</v>
+        <v>149</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D17" s="6"/>
+        <v>124</v>
+      </c>
+      <c r="D17" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>182</v>
+        <v>150</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>249</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>183</v>
+        <v>151</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>188</v>
+        <v>156</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>251</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>189</v>
+        <v>157</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>192</v>
+        <v>160</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B33" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B35" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>198</v>
+        <v>166</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>201</v>
+        <v>169</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>200</v>
+        <v>168</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>210</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>206</v>
+        <v>184</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>174</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>206</v>
+        <v>214</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>174</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>206</v>
+        <v>163</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>174</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>197</v>
+        <v>165</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new stimulus information
</commit_message>
<xml_diff>
--- a/dataDefinitions.xlsx
+++ b/dataDefinitions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspaces\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97CA96D-A8CD-4153-AA9C-BADB711B8038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD68674-64EC-466B-9885-3F2D990D8DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3F3756E1-F16D-4C67-A02C-119F78A23B8F}"/>
+    <workbookView xWindow="6240" yWindow="810" windowWidth="18615" windowHeight="12825" activeTab="3" xr2:uid="{3F3756E1-F16D-4C67-A02C-119F78A23B8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Imaging" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="263">
   <si>
     <t>File name</t>
   </si>
@@ -784,6 +784,51 @@
   </si>
   <si>
     <t>Sixe of pxiels in mm</t>
+  </si>
+  <si>
+    <t>gratingsStep.startTime</t>
+  </si>
+  <si>
+    <t>gratingsStep.endTime</t>
+  </si>
+  <si>
+    <t>gratingsStep.direction</t>
+  </si>
+  <si>
+    <t>gratingsStep.spatialF</t>
+  </si>
+  <si>
+    <t>gratingsStep.contrast</t>
+  </si>
+  <si>
+    <t>gratingsStepExp.intervals</t>
+  </si>
+  <si>
+    <t>gratingsStep.startTemporalF</t>
+  </si>
+  <si>
+    <t>gratingsStep.endTemporalF</t>
+  </si>
+  <si>
+    <t>initial temporal frequency</t>
+  </si>
+  <si>
+    <t>final temporal frequency</t>
+  </si>
+  <si>
+    <t>flicker.startTime</t>
+  </si>
+  <si>
+    <t>flicker.endTime</t>
+  </si>
+  <si>
+    <t>flicker.contrast</t>
+  </si>
+  <si>
+    <t>block contrast (Low or High)</t>
+  </si>
+  <si>
+    <t>flickerExp.intervals</t>
   </si>
 </sst>
 </file>
@@ -968,9 +1013,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1008,7 +1053,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1114,7 +1159,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1256,7 +1301,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1882,7 +1927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBC7223-8FD1-49F7-AA31-6BD218EA8AEE}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
@@ -2023,16 +2068,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F47D32-613F-478F-B67D-600975316B20}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" style="1" customWidth="1"/>
     <col min="2" max="3" width="16.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="110.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="157.42578125" style="1" customWidth="1"/>
@@ -2372,6 +2417,174 @@
         <v>222</v>
       </c>
       <c r="D27" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>223</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed correction of z motion correction
Changed the way bad frames are removed.
Now based on higher and lower fluoresence in different ends of the plane
</commit_message>
<xml_diff>
--- a/dataDefinitions.xlsx
+++ b/dataDefinitions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD68674-64EC-466B-9885-3F2D990D8DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B7778C-4101-4523-8E90-3D40CEE78C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="810" windowWidth="18615" windowHeight="12825" activeTab="3" xr2:uid="{3F3756E1-F16D-4C67-A02C-119F78A23B8F}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{3F3756E1-F16D-4C67-A02C-119F78A23B8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Imaging" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="277">
   <si>
     <t>File name</t>
   </si>
@@ -829,6 +829,48 @@
   </si>
   <si>
     <t>flickerExp.intervals</t>
+  </si>
+  <si>
+    <t>circlesResp.map</t>
+  </si>
+  <si>
+    <t>nUnits, t,y,x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The average response in each square </t>
+  </si>
+  <si>
+    <t>nUnits,diameters,y,x</t>
+  </si>
+  <si>
+    <t>The maps divided by the size of the circles</t>
+  </si>
+  <si>
+    <t>The maps divided by the size of the circles, the average map was taken considerin not only the centres, but also any circle part touching each point</t>
+  </si>
+  <si>
+    <t>circlesRF.maps</t>
+  </si>
+  <si>
+    <t>circlesRF.mapsDiameters</t>
+  </si>
+  <si>
+    <t>circleAnalysis.resp.timestamps</t>
+  </si>
+  <si>
+    <t>1,t</t>
+  </si>
+  <si>
+    <t>the time stamps for circleResp.map</t>
+  </si>
+  <si>
+    <t>1,nDiameters</t>
+  </si>
+  <si>
+    <t>the diameters used in fitting</t>
+  </si>
+  <si>
+    <t>circleAnalysis.size.diameters</t>
   </si>
 </sst>
 </file>
@@ -1312,8 +1354,8 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,7 +1971,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,9 +2112,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F47D32-613F-478F-B67D-600975316B20}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2595,11 +2637,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DAE84D7-1D35-455E-9EAE-38426D5ED717}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3003,51 +3045,37 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>174</v>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>121</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>121</v>
@@ -3056,12 +3084,12 @@
         <v>169</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>121</v>
@@ -3070,91 +3098,175 @@
         <v>169</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>121</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>181</v>
+        <v>269</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>169</v>
+        <v>266</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>182</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>204</v>
+        <v>270</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>244</v>
+        <v>266</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>240</v>
+        <v>268</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>121</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>241</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>121</v>
+        <v>171</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>169</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>242</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added SC channel definition
</commit_message>
<xml_diff>
--- a/dataDefinitions.xlsx
+++ b/dataDefinitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspaces\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA141186-DC26-4564-B86A-41053D9688FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4430D0-E227-4164-8957-C66690F8EE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="4" xr2:uid="{3F3756E1-F16D-4C67-A02C-119F78A23B8F}"/>
+    <workbookView xWindow="-1958" yWindow="-16297" windowWidth="28995" windowHeight="15675" activeTab="1" xr2:uid="{3F3756E1-F16D-4C67-A02C-119F78A23B8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Imaging" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="351">
   <si>
     <t>File name</t>
   </si>
@@ -1084,6 +1084,15 @@
   </si>
   <si>
     <t>nUnits(# neurons): neuron ID;  nStimID: F1 value per direction</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>Channels along probe coinciding with (1) the top of SC, and (2) the border between SGS and SO</t>
+  </si>
+  <si>
+    <t>recording.scChannels</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1217,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1248,9 +1257,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1576,16 +1582,16 @@
       <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.46484375" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="157.44140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="3" max="3" width="20.86328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="157.46484375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1599,7 +1605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
@@ -1613,7 +1619,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>17</v>
       </c>
@@ -1627,11 +1633,11 @@
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="11"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>22</v>
       </c>
@@ -1645,7 +1651,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>283</v>
       </c>
@@ -1659,7 +1665,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1673,7 +1679,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>19</v>
       </c>
@@ -1687,7 +1693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1701,7 +1707,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>20</v>
       </c>
@@ -1715,7 +1721,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>21</v>
       </c>
@@ -1729,7 +1735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>290</v>
       </c>
@@ -1743,7 +1749,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>179</v>
       </c>
@@ -1757,7 +1763,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>205</v>
       </c>
@@ -1771,7 +1777,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>303</v>
       </c>
@@ -1785,7 +1791,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>305</v>
       </c>
@@ -1799,7 +1805,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>307</v>
       </c>
@@ -1813,7 +1819,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>308</v>
       </c>
@@ -1827,7 +1833,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>311</v>
       </c>
@@ -1841,7 +1847,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>313</v>
       </c>
@@ -1855,20 +1861,20 @@
         <v>314</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -1882,7 +1888,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>37</v>
       </c>
@@ -1901,23 +1907,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB1A0A7-F272-47D7-84D8-7D69F6A764BE}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.46484375" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="157.44140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="3" max="3" width="20.86328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="157.46484375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1931,7 +1937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>99</v>
       </c>
@@ -1945,7 +1951,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>100</v>
       </c>
@@ -1959,7 +1965,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>101</v>
       </c>
@@ -1973,7 +1979,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>106</v>
       </c>
@@ -1987,7 +1993,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>110</v>
       </c>
@@ -2001,7 +2007,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>112</v>
       </c>
@@ -2015,7 +2021,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>113</v>
       </c>
@@ -2029,13 +2035,13 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
@@ -2049,7 +2055,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
@@ -2063,7 +2069,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
@@ -2077,7 +2083,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -2091,7 +2097,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>54</v>
       </c>
@@ -2105,10 +2111,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
@@ -2122,7 +2128,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -2136,7 +2142,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
@@ -2150,7 +2156,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>59</v>
       </c>
@@ -2164,7 +2170,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -2178,7 +2184,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -2192,7 +2198,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
@@ -2206,7 +2212,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>77</v>
       </c>
@@ -2220,7 +2226,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -2234,7 +2240,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
@@ -2248,7 +2254,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>70</v>
       </c>
@@ -2262,7 +2268,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>46</v>
       </c>
@@ -2276,7 +2282,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>74</v>
       </c>
@@ -2288,6 +2294,20 @@
       </c>
       <c r="D30" s="1" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -2305,16 +2325,16 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.46484375" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="157.44140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="3" max="3" width="20.86328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="157.46484375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2328,7 +2348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>212</v>
       </c>
@@ -2342,7 +2362,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>272</v>
       </c>
@@ -2356,11 +2376,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>80</v>
       </c>
@@ -2374,7 +2394,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>81</v>
       </c>
@@ -2388,7 +2408,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>274</v>
       </c>
@@ -2402,7 +2422,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>240</v>
       </c>
@@ -2416,11 +2436,11 @@
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>286</v>
       </c>
@@ -2434,7 +2454,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>288</v>
       </c>
@@ -2448,7 +2468,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>273</v>
       </c>
@@ -2476,16 +2496,16 @@
       <selection pane="bottomLeft" activeCell="B53" sqref="A53:B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.86328125" style="1" customWidth="1"/>
     <col min="2" max="3" width="16.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="110.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="157.44140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="5" max="5" width="157.46484375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2499,7 +2519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>201</v>
       </c>
@@ -2513,7 +2533,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>202</v>
       </c>
@@ -2527,7 +2547,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>213</v>
       </c>
@@ -2541,7 +2561,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>183</v>
       </c>
@@ -2555,7 +2575,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>184</v>
       </c>
@@ -2569,7 +2589,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>185</v>
       </c>
@@ -2583,7 +2603,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>278</v>
       </c>
@@ -2597,7 +2617,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>280</v>
       </c>
@@ -2611,7 +2631,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>216</v>
       </c>
@@ -2625,7 +2645,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>214</v>
       </c>
@@ -2639,7 +2659,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>214</v>
       </c>
@@ -2653,7 +2673,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>186</v>
       </c>
@@ -2667,7 +2687,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>215</v>
       </c>
@@ -2681,7 +2701,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>219</v>
       </c>
@@ -2695,7 +2715,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>220</v>
       </c>
@@ -2709,7 +2729,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>221</v>
       </c>
@@ -2723,7 +2743,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>222</v>
       </c>
@@ -2737,7 +2757,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
         <v>223</v>
       </c>
@@ -2751,7 +2771,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>203</v>
       </c>
@@ -2765,7 +2785,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>204</v>
       </c>
@@ -2779,7 +2799,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>191</v>
       </c>
@@ -2793,7 +2813,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>193</v>
       </c>
@@ -2807,7 +2827,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>194</v>
       </c>
@@ -2821,7 +2841,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>196</v>
       </c>
@@ -2835,7 +2855,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>276</v>
       </c>
@@ -2849,7 +2869,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="5" t="s">
         <v>224</v>
       </c>
@@ -2863,7 +2883,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>243</v>
       </c>
@@ -2877,7 +2897,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>244</v>
       </c>
@@ -2891,7 +2911,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>245</v>
       </c>
@@ -2905,7 +2925,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>246</v>
       </c>
@@ -2919,7 +2939,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>249</v>
       </c>
@@ -2933,7 +2953,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>250</v>
       </c>
@@ -2947,7 +2967,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>247</v>
       </c>
@@ -2961,7 +2981,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="5" t="s">
         <v>248</v>
       </c>
@@ -2975,7 +2995,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>253</v>
       </c>
@@ -2989,7 +3009,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>254</v>
       </c>
@@ -3003,7 +3023,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>255</v>
       </c>
@@ -3017,7 +3037,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="5" t="s">
         <v>257</v>
       </c>
@@ -3031,7 +3051,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>293</v>
       </c>
@@ -3045,7 +3065,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>294</v>
       </c>
@@ -3059,7 +3079,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>295</v>
       </c>
@@ -3073,7 +3093,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A51" s="5" t="s">
         <v>299</v>
       </c>
@@ -3087,7 +3107,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="5" t="s">
         <v>298</v>
       </c>
@@ -3110,21 +3130,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DAE84D7-1D35-455E-9EAE-38426D5ED717}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="43.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="157.44140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="3" max="3" width="20.86328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="157.46484375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3138,7 +3158,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>116</v>
       </c>
@@ -3152,7 +3172,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>119</v>
       </c>
@@ -3166,13 +3186,13 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>132</v>
       </c>
@@ -3186,7 +3206,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>133</v>
       </c>
@@ -3200,7 +3220,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>134</v>
       </c>
@@ -3214,7 +3234,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>135</v>
       </c>
@@ -3228,7 +3248,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>136</v>
       </c>
@@ -3242,7 +3262,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>137</v>
       </c>
@@ -3256,13 +3276,13 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>138</v>
       </c>
@@ -3276,7 +3296,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>139</v>
       </c>
@@ -3288,7 +3308,7 @@
       </c>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>140</v>
       </c>
@@ -3300,7 +3320,7 @@
       </c>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>141</v>
       </c>
@@ -3312,7 +3332,7 @@
       </c>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>142</v>
       </c>
@@ -3323,7 +3343,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>143</v>
       </c>
@@ -3335,7 +3355,7 @@
       </c>
       <c r="D17" s="4"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>144</v>
       </c>
@@ -3349,7 +3369,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>145</v>
       </c>
@@ -3360,7 +3380,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>146</v>
       </c>
@@ -3371,7 +3391,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>147</v>
       </c>
@@ -3382,7 +3402,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>148</v>
       </c>
@@ -3393,7 +3413,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>149</v>
       </c>
@@ -3404,7 +3424,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>150</v>
       </c>
@@ -3418,7 +3438,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>151</v>
       </c>
@@ -3429,7 +3449,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>152</v>
       </c>
@@ -3440,7 +3460,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>153</v>
       </c>
@@ -3451,7 +3471,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>154</v>
       </c>
@@ -3462,7 +3482,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
         <v>155</v>
       </c>
@@ -3474,7 +3494,7 @@
       </c>
       <c r="D31" s="5"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>129</v>
       </c>
@@ -3488,7 +3508,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>130</v>
       </c>
@@ -3502,7 +3522,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>131</v>
       </c>
@@ -3516,7 +3536,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>258</v>
       </c>
@@ -3530,7 +3550,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>160</v>
       </c>
@@ -3544,7 +3564,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>161</v>
       </c>
@@ -3558,7 +3578,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>163</v>
       </c>
@@ -3572,7 +3592,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>162</v>
       </c>
@@ -3586,7 +3606,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>164</v>
       </c>
@@ -3600,7 +3620,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>264</v>
       </c>
@@ -3614,7 +3634,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>265</v>
       </c>
@@ -3628,7 +3648,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>156</v>
       </c>
@@ -3642,7 +3662,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>177</v>
       </c>
@@ -3656,7 +3676,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>200</v>
       </c>
@@ -3670,7 +3690,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>157</v>
       </c>
@@ -3684,7 +3704,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>158</v>
       </c>
@@ -3698,7 +3718,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>159</v>
       </c>
@@ -3712,7 +3732,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>266</v>
       </c>
@@ -3726,7 +3746,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>271</v>
       </c>
@@ -3740,7 +3760,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="14" t="s">
         <v>315</v>
       </c>
@@ -3754,7 +3774,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>318</v>
       </c>
@@ -3768,7 +3788,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>320</v>
       </c>
@@ -3782,7 +3802,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>322</v>
       </c>
@@ -3796,7 +3816,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>324</v>
       </c>
@@ -3810,7 +3830,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>327</v>
       </c>
@@ -3824,7 +3844,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>329</v>
       </c>
@@ -3838,7 +3858,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>331</v>
       </c>
@@ -3852,7 +3872,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>333</v>
       </c>
@@ -3866,7 +3886,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>336</v>
       </c>
@@ -3880,36 +3900,36 @@
         <v>339</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="15" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A67" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="B67" s="15" t="s">
+      <c r="B67" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="C67" s="15" t="s">
+      <c r="C67" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D67" s="15" t="s">
+      <c r="D67" s="1" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="68" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="15" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A68" s="1" t="s">
         <v>343</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C68" s="15" t="s">
+      <c r="C68" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="D68" s="15" t="s">
+      <c r="D68" s="1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="15" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A69" s="1" t="s">
         <v>344</v>
       </c>
       <c r="B69" s="1" t="s">

</xml_diff>